<commit_message>
Basing functionality of the application completed: Controlling tuner works;  Tuner mode works; Reading SWR should work;
</commit_message>
<xml_diff>
--- a/docs/ATU_SerialProtocol.xlsx
+++ b/docs/ATU_SerialProtocol.xlsx
@@ -165,9 +165,6 @@
     <t>Lo/Hi L</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -237,6 +234,9 @@
   </si>
   <si>
     <t xml:space="preserve">C2 active :   L14 = 1, CM1 = 0 </t>
+  </si>
+  <si>
+    <t>L  (bits should be inverted)</t>
   </si>
 </sst>
 </file>
@@ -367,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -379,6 +379,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,7 +699,7 @@
   <dimension ref="A1:AI21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AI7" sqref="AI7"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -718,105 +721,105 @@
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:35" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="H4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="J4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="L4" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="M4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="N4" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="O4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="P4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="Q4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="Q4" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="S4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="T4" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="T4" s="10" t="s">
+      <c r="U4" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="V4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="10" t="s">
+      <c r="W4" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="W4" s="10" t="s">
+      <c r="X4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="X4" s="10" t="s">
+      <c r="Y4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="Y4" s="10" t="s">
+      <c r="Z4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="Z4" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="AB4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC4" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="AC4" s="10" t="s">
+      <c r="AD4" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="AD4" s="10" t="s">
+      <c r="AE4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="AE4" s="10" t="s">
+      <c r="AF4" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="AF4" s="10" t="s">
+      <c r="AG4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="AG4" s="10" t="s">
+      <c r="AH4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="AH4" s="10" t="s">
+      <c r="AI4" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="AI4" s="10" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -919,7 +922,7 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -934,7 +937,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="2" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
@@ -962,39 +965,42 @@
         <v>34</v>
       </c>
     </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AI7" s="11"/>
+    </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.35">
       <c r="I10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="G14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="G15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>